<commit_message>
fixing relevant tickets / v.5
</commit_message>
<xml_diff>
--- a/beta_version/excel_files/testing.xlsx
+++ b/beta_version/excel_files/testing.xlsx
@@ -390,7 +390,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:H19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -567,6 +567,584 @@
         </is>
       </c>
     </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>WC48 P5F</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>AOI (malla)</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>2024-06-05</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>09:12:53</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>09:12:54</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>0:00:01</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>WC48 P5F</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Cámara no detecta busbar</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>2024-06-05</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>09:13:01</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>09:13:02</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>0:00:01</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>WC48 P5F</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>AOI (malla)</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>2024-06-05</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>09:13:09</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>09:13:09</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>0:00:00</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>0.14 minutos</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>WV50 FILTER</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>NOK Soldadura Plástico</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>2024-06-05</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>09:17:50</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>WV50 FILTER</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>NOK Soldad. Plástico+Metal</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>2024-06-05</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>09:20:14</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>09:20:16</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>0:00:02</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>WV50 FILTER</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>No coloca bien la pcb</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>2024-06-05</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>09:20:24</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>09:20:25</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>0:00:01</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>WV50 FILTER</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Fallo atornillador</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>2024-06-05</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>09:20:30</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>09:20:31</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>0:00:01</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>0.16 minutos</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>WV50 FILTER</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>NOK Soldad. Plástico+Metal</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>2024-06-05</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>09:20:38</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>09:20:38</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>0:00:00</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>0.13 minutos</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>WV50 FILTER</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Fallo cámara ferrite</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>2024-06-05</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>09:21:05</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>09:21:05</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>0:00:00</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>0.13 minutos</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>WV50 FILTER</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Traza</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>2024-06-05</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>09:21:53</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>09:21:54</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>0:00:01</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>WV50 FILTER</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Traza</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>2024-06-05</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>09:27:10</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>09:27:11</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>0:00:01</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>WV50 FILTER</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>QR desplazado</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>2024-06-05</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>09:27:14</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>09:27:15</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>0:00:01</t>
+        </is>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>WV50 FILTER</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Fallo atornillador</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>2024-06-05</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>09:27:20</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>09:27:21</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>0:00:01</t>
+        </is>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>0.07 minutos</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>WV50 FILTER</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>Fallo atornillador</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>2024-06-05</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>09:27:23</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>09:27:24</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>0:00:01</t>
+        </is>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>0.08 minutos</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
fixing errors and bugs from mtbf / v.5.5
</commit_message>
<xml_diff>
--- a/beta_version/excel_files/testing.xlsx
+++ b/beta_version/excel_files/testing.xlsx
@@ -390,7 +390,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H19"/>
+  <dimension ref="A1:H24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1145,6 +1145,216 @@
         </is>
       </c>
     </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>WV50 FILTER</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>NOK Soldadura metal</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>2024-06-05</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>09:34:16</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>09:34:16</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>0:00:00</t>
+        </is>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>WV50 FILTER</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>No coloca bien la pcb</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>2024-06-05</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>09:34:24</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>09:34:25</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>0:00:01</t>
+        </is>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>WV50 FILTER</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>Robot no coloca bien ferrita</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>2024-06-05</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>09:34:53</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>09:34:53</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>0:00:00</t>
+        </is>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>0.15 minutos</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>WV50 FILTER</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>Traza</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>2024-06-05</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>09:41:53</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>09:41:54</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>0:00:01</t>
+        </is>
+      </c>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>WV50 FILTER</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>NOK Soldadura metal</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>2024-06-05</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>09:42:10</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>09:42:11</t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>0:00:01</t>
+        </is>
+      </c>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
issues __init__ / class / v.6.1
</commit_message>
<xml_diff>
--- a/beta_version/excel_files/testing.xlsx
+++ b/beta_version/excel_files/testing.xlsx
@@ -390,7 +390,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H24"/>
+  <dimension ref="A1:H30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1355,6 +1355,258 @@
         </is>
       </c>
     </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>WC47 NACP</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>Fallo tolva</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>2024-06-05</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>10:48:47</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>10:48:48</t>
+        </is>
+      </c>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>0:00:01</t>
+        </is>
+      </c>
+      <c r="H25" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>WC47 NACP</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>No coge placa</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>2024-06-05</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>10:48:49</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>10:48:50</t>
+        </is>
+      </c>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>0:00:01</t>
+        </is>
+      </c>
+      <c r="H26" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>WC47 NACP</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>Fallo en elevador</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>2024-06-05</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>10:48:52</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>10:48:52</t>
+        </is>
+      </c>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>0:00:00</t>
+        </is>
+      </c>
+      <c r="H27" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>WC48 P5F</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>AOI (fallo etiqueta)</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>2024-06-05</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>10:50:52</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>10:50:53</t>
+        </is>
+      </c>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t>0:00:01</t>
+        </is>
+      </c>
+      <c r="H28" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>WC48 P5F</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>Cámara no detecta Pcb</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>2024-06-05</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>10:50:54</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>10:50:57</t>
+        </is>
+      </c>
+      <c r="G29" t="inlineStr">
+        <is>
+          <t>0:00:03</t>
+        </is>
+      </c>
+      <c r="H29" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>WC48 P5F</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>No detecta presencia power CP</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>2024-06-05</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>10:50:56</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>10:50:57</t>
+        </is>
+      </c>
+      <c r="G30" t="inlineStr">
+        <is>
+          <t>0:00:01</t>
+        </is>
+      </c>
+      <c r="H30" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>